<commit_message>
updated manual testing excel and added R5into Readme
</commit_message>
<xml_diff>
--- a/public/User Acceptance Testing.xlsx
+++ b/public/User Acceptance Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anawang/Desktop/My life in Tech/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4379A131-CA9A-7049-88F2-171834ADE037}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{518129BF-03E3-E741-BFCF-8D803C7BA56F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="0" windowWidth="32000" windowHeight="18000" xr2:uid="{5771E9D7-2C04-E14D-9FEA-95E6E4571377}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="121">
   <si>
     <t>Test Case</t>
   </si>
@@ -285,9 +285,6 @@
     <t>✅With my manager account, I can change all the information of the ticket that belongs to other people.</t>
   </si>
   <si>
-    <t>Chen fixed the edit button for managers on 19 Nov 2022. Now managers can only edit the confidence, efoort, and impact values from other people's tickets</t>
-  </si>
-  <si>
     <t>I cannot edit other people's confidence, effort, and impact values.</t>
   </si>
   <si>
@@ -321,9 +318,6 @@
     <t>I cannot view or edit my profile</t>
   </si>
   <si>
-    <t>We need to allow users to edit their manager/employee status in the future</t>
-  </si>
-  <si>
     <t>✅ I cannot manage my manager status in the my user profile page.</t>
   </si>
   <si>
@@ -382,6 +376,18 @@
   </si>
   <si>
     <t>We should enable users to search for the relevant conetxt without concerning capital word spellings in the future.</t>
+  </si>
+  <si>
+    <t>✅ I noticed that the managers can view the feedback but the employees cannot. Our team members should be able to view my feedback.</t>
+  </si>
+  <si>
+    <t>We should enable users to view their manager's feedback in the future.</t>
+  </si>
+  <si>
+    <t>Chen fixed the edit button for managers on 19 Nov 2022. Now managers can only edit the confidence, effort, and impact values from other people's tickets</t>
+  </si>
+  <si>
+    <t>We need to allow users to edit their manager/employee status in their profile page in the future.</t>
   </si>
 </sst>
 </file>
@@ -548,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -639,6 +645,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79B8DB3-DF16-F946-A557-108DFA618EAF}">
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -977,7 +986,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1088,10 +1097,10 @@
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>4</v>
@@ -1610,7 +1619,7 @@
         <v>82</v>
       </c>
       <c r="F45" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1698,10 +1707,10 @@
     <row r="52" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>4</v>
@@ -1710,7 +1719,7 @@
         <v>85</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1726,22 +1735,22 @@
     <row r="54" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E54" s="13"/>
       <c r="F54" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>41</v>
@@ -1754,28 +1763,28 @@
     <row r="56" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="26"/>
       <c r="B56" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D56" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="26"/>
       <c r="B57" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="23" t="s">
         <v>94</v>
-      </c>
-      <c r="C57" s="23" t="s">
-        <v>95</v>
       </c>
       <c r="D57" s="23" t="s">
         <v>4</v>
@@ -1798,10 +1807,10 @@
     <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="27"/>
       <c r="B59" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="23" t="s">
         <v>96</v>
-      </c>
-      <c r="C59" s="23" t="s">
-        <v>97</v>
       </c>
       <c r="D59" s="23" t="s">
         <v>4</v>
@@ -1811,7 +1820,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>41</v>
@@ -1824,10 +1833,10 @@
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="30"/>
       <c r="B61" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D61" s="23" t="s">
         <v>4</v>
@@ -1840,10 +1849,10 @@
     <row r="62" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="30"/>
       <c r="B62" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D62" s="23" t="s">
         <v>4</v>
@@ -1856,44 +1865,46 @@
     <row r="63" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A63" s="30"/>
       <c r="B63" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C63" s="23" t="s">
-        <v>106</v>
-      </c>
       <c r="D63" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F63" s="23" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A64" s="30"/>
       <c r="B64" s="23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D64" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F64" s="28"/>
+        <v>117</v>
+      </c>
+      <c r="F64" s="33" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="30"/>
       <c r="B65" s="23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D65" s="23" t="s">
         <v>4</v>
@@ -1916,10 +1927,10 @@
     <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="31"/>
       <c r="B67" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D67" s="23" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
added more feature into manual testing
</commit_message>
<xml_diff>
--- a/public/User Acceptance Testing.xlsx
+++ b/public/User Acceptance Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anawang/Desktop/My life in Tech/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{518129BF-03E3-E741-BFCF-8D803C7BA56F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{812B9839-A9D6-3A45-9C26-DD1D9EE49725}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="32000" windowHeight="18000" xr2:uid="{5771E9D7-2C04-E14D-9FEA-95E6E4571377}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="32000" windowHeight="17540" xr2:uid="{5771E9D7-2C04-E14D-9FEA-95E6E4571377}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="126">
   <si>
     <t>Test Case</t>
   </si>
@@ -378,16 +378,31 @@
     <t>We should enable users to search for the relevant conetxt without concerning capital word spellings in the future.</t>
   </si>
   <si>
-    <t>✅ I noticed that the managers can view the feedback but the employees cannot. Our team members should be able to view my feedback.</t>
-  </si>
-  <si>
-    <t>We should enable users to view their manager's feedback in the future.</t>
-  </si>
-  <si>
     <t>Chen fixed the edit button for managers on 19 Nov 2022. Now managers can only edit the confidence, effort, and impact values from other people's tickets</t>
   </si>
   <si>
-    <t>We need to allow users to edit their manager/employee status in their profile page in the future.</t>
+    <t>✅As managers, we want to be able to delete the submitted tickets that are no longer useful/meaningful.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can build admin account to allow managers to delete the submitted tickets in the future. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can build admin account to allow managers to edit manager/employee status in the future. </t>
+  </si>
+  <si>
+    <t>When I log into my account, I can view MyTickets listing page</t>
+  </si>
+  <si>
+    <t>I am able to view all my tickets that are created or saved before.</t>
+  </si>
+  <si>
+    <t>It redirects me to the ticket deails page to view the feedback</t>
+  </si>
+  <si>
+    <t>I cannot view my feedback</t>
+  </si>
+  <si>
+    <t>Enable users to view their manager's feedback</t>
   </si>
 </sst>
 </file>
@@ -554,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -562,13 +577,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -578,44 +587,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -624,6 +600,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -633,7 +616,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -643,11 +631,50 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -968,15 +995,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79B8DB3-DF16-F946-A557-108DFA618EAF}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" style="9" customWidth="1"/>
     <col min="2" max="2" width="59.83203125" customWidth="1"/>
     <col min="3" max="3" width="58.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
@@ -1005,751 +1032,753 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="7"/>
+      <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="7"/>
+      <c r="D5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="7"/>
+      <c r="D6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="7"/>
+      <c r="D7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="32"/>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="7"/>
+      <c r="D9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="29"/>
+      <c r="B10" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="7"/>
+      <c r="D11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="29"/>
+      <c r="B13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="7"/>
+      <c r="D13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="D14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="12" t="s">
+      <c r="D15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="29"/>
+      <c r="B16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="7"/>
+      <c r="D16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="29"/>
+      <c r="B17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="7"/>
+      <c r="D17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="29"/>
+      <c r="B18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="7"/>
+      <c r="D18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="29"/>
+      <c r="B19" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="28"/>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="29"/>
+      <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="7"/>
+      <c r="D20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="25"/>
     </row>
     <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="33"/>
+      <c r="B22" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="7"/>
+      <c r="D22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="33"/>
+      <c r="B23" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="6" t="s">
+      <c r="D23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6" t="s">
+      <c r="A24" s="33"/>
+      <c r="B24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="7"/>
+      <c r="D24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="119" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="33"/>
+      <c r="B25" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="D25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="15" t="s">
+      <c r="A26" s="33"/>
+      <c r="B26" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="17"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="28"/>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6" t="s">
+      <c r="A27" s="33"/>
+      <c r="B27" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="6"/>
+      <c r="D27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6" t="s">
+      <c r="A28" s="33"/>
+      <c r="B28" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="6" t="s">
+      <c r="D28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="4" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="25"/>
     </row>
     <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="6" t="s">
+      <c r="A30" s="29"/>
+      <c r="B30" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="7"/>
+      <c r="D30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="6" t="s">
+      <c r="A31" s="29"/>
+      <c r="B31" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="7"/>
+      <c r="D31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="15" t="s">
+      <c r="A32" s="29"/>
+      <c r="B32" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="17"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="28"/>
     </row>
     <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="6" t="s">
+      <c r="A33" s="29"/>
+      <c r="B33" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="7"/>
+      <c r="D33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="21"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="25"/>
     </row>
     <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="6" t="s">
+      <c r="A35" s="29"/>
+      <c r="B35" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="7"/>
+      <c r="D35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="6" t="s">
+      <c r="A36" s="29"/>
+      <c r="B36" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="7"/>
+      <c r="D36" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="15" t="s">
+      <c r="A37" s="29"/>
+      <c r="B37" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="17"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="28"/>
     </row>
     <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="6" t="s">
+      <c r="A38" s="29"/>
+      <c r="B38" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="7"/>
+      <c r="D38" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="21"/>
-    </row>
-    <row r="40" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="6" t="s">
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="25"/>
+    </row>
+    <row r="40" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A40" s="29"/>
+      <c r="B40" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="7"/>
+      <c r="D40" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F40" s="34" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="6" t="s">
+      <c r="A41" s="29"/>
+      <c r="B41" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F41" s="7"/>
+      <c r="D41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="15" t="s">
+      <c r="A42" s="29"/>
+      <c r="B42" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="17"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="28"/>
     </row>
     <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="6" t="s">
+      <c r="A43" s="29"/>
+      <c r="B43" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="12"/>
-      <c r="F43" s="7"/>
+      <c r="D43" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="7"/>
+      <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="21"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="25"/>
     </row>
     <row r="45" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="6" t="s">
+      <c r="A45" s="29"/>
+      <c r="B45" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" s="12" t="s">
+      <c r="D45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F45" s="32" t="s">
+      <c r="F45" s="13" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="15" t="s">
+      <c r="A46" s="29"/>
+      <c r="B46" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="17"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="28"/>
     </row>
     <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="6" t="s">
+      <c r="A47" s="29"/>
+      <c r="B47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E47" s="12"/>
-      <c r="F47" s="7"/>
+      <c r="D47" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="7"/>
+      <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="6" t="s">
+      <c r="A48" s="29"/>
+      <c r="B48" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E48" s="12"/>
-      <c r="F48" s="7"/>
+      <c r="D48" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="7"/>
+      <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B49" s="19" t="s">
+      <c r="B49" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="21"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="25"/>
     </row>
     <row r="50" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="6" t="s">
+      <c r="A50" s="29"/>
+      <c r="B50" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D50" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" s="7"/>
+      <c r="D50" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="6" t="s">
+      <c r="A51" s="29"/>
+      <c r="B51" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" s="7"/>
+      <c r="D51" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
-      <c r="B52" s="6" t="s">
+      <c r="A52" s="29"/>
+      <c r="B52" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D52" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E52" s="12" t="s">
+      <c r="D52" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F52" s="6" t="s">
-        <v>119</v>
+      <c r="F52" s="4" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
-      <c r="B53" s="15" t="s">
+      <c r="A53" s="29"/>
+      <c r="B53" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="17"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="28"/>
     </row>
     <row r="54" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="6" t="s">
+      <c r="A54" s="29"/>
+      <c r="B54" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D54" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E54" s="13"/>
-      <c r="F54" s="6" t="s">
+      <c r="D54" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="8"/>
+      <c r="F54" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="25" t="s">
+      <c r="A55" s="15" t="s">
         <v>91</v>
       </c>
       <c r="B55" s="18" t="s">
@@ -1760,66 +1789,66 @@
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
     </row>
-    <row r="56" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A56" s="26"/>
-      <c r="B56" s="23" t="s">
+    <row r="56" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A56" s="16"/>
+      <c r="B56" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C56" s="23" t="s">
+      <c r="C56" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D56" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E56" s="12" t="s">
+      <c r="D56" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F56" s="23" t="s">
+      <c r="F56" s="34" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="26"/>
-      <c r="B57" s="23" t="s">
+      <c r="A57" s="16"/>
+      <c r="B57" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C57" s="23" t="s">
+      <c r="C57" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D57" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57" s="4"/>
+      <c r="D57" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="26"/>
-      <c r="B58" s="14" t="s">
+      <c r="A58" s="16"/>
+      <c r="B58" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
     </row>
     <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="27"/>
-      <c r="B59" s="6" t="s">
+      <c r="A59" s="17"/>
+      <c r="B59" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C59" s="23" t="s">
+      <c r="C59" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D59" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E59" s="24"/>
-      <c r="F59" s="4"/>
+      <c r="D59" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" s="11"/>
+      <c r="F59" s="3"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="29" t="s">
+      <c r="A60" s="20" t="s">
         <v>109</v>
       </c>
       <c r="B60" s="18" t="s">
@@ -1831,130 +1860,185 @@
       <c r="F60" s="18"/>
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="30"/>
-      <c r="B61" s="23" t="s">
+      <c r="A61" s="21"/>
+      <c r="B61" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C61" s="23" t="s">
+      <c r="C61" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D61" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F61" s="28"/>
+      <c r="D61" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="12"/>
     </row>
     <row r="62" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A62" s="30"/>
-      <c r="B62" s="23" t="s">
+      <c r="A62" s="21"/>
+      <c r="B62" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C62" s="23" t="s">
+      <c r="C62" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="D62" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F62" s="28"/>
+      <c r="D62" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="12"/>
     </row>
     <row r="63" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A63" s="30"/>
-      <c r="B63" s="23" t="s">
+      <c r="A63" s="21"/>
+      <c r="B63" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C63" s="23" t="s">
+      <c r="C63" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D63" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E63" s="12" t="s">
+      <c r="D63" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F63" s="23" t="s">
+      <c r="F63" s="34" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="119" x14ac:dyDescent="0.2">
-      <c r="A64" s="30"/>
-      <c r="B64" s="23" t="s">
+    <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="21"/>
+      <c r="B64" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C64" s="23" t="s">
+      <c r="C64" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D64" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="F64" s="33" t="s">
-        <v>118</v>
-      </c>
+      <c r="D64" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="14"/>
     </row>
     <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="30"/>
-      <c r="B65" s="23" t="s">
+      <c r="A65" s="21"/>
+      <c r="B65" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C65" s="23" t="s">
+      <c r="C65" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D65" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F65" s="28"/>
+      <c r="D65" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" s="12"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="30"/>
-      <c r="B66" s="14" t="s">
+      <c r="A66" s="21"/>
+      <c r="B66" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
     </row>
     <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="31"/>
-      <c r="B67" s="6" t="s">
+      <c r="A67" s="22"/>
+      <c r="B67" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C67" s="23" t="s">
+      <c r="C67" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D67" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E67" s="24"/>
-      <c r="F67" s="28"/>
+      <c r="D67" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" s="11"/>
+      <c r="F67" s="12"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+    </row>
+    <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="36"/>
+      <c r="B69" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="12"/>
+    </row>
+    <row r="70" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="36"/>
+      <c r="B70" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" s="12"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="36"/>
+      <c r="B71" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+    </row>
+    <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" s="37"/>
+      <c r="B72" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" s="11"/>
+      <c r="F72" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A55:A59"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="A60:A67"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B39:F39"/>
+  <mergeCells count="35">
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="A68:A72"/>
     <mergeCell ref="B42:F42"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A49:A54"/>
@@ -1971,7 +2055,21 @@
     <mergeCell ref="A21:A28"/>
     <mergeCell ref="A29:A33"/>
     <mergeCell ref="A34:A38"/>
-    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="A60:A67"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B58:F58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>